<commit_message>
Add MNI current meter LL conversion
</commit_message>
<xml_diff>
--- a/data/ROV_lat_conv.xlsx
+++ b/data/ROV_lat_conv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc504838/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc504838/Science/Data &amp; analysis/GeoWrangling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A41ECC5-6369-8442-94CD-D1CC277A20B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BE0209-562E-844C-8085-46A0C3A8AC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,16 +769,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1232,13 +1229,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2:K72"/>
+      <selection pane="bottomRight" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,23 +1290,23 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="6">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2">
         <v>44389</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2" t="s">
@@ -1324,7 +1321,7 @@
       <c r="K2">
         <v>150.79887390136699</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1437,10 +1434,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="2">
         <v>44393</v>
       </c>
@@ -1569,10 +1566,10 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="2">
         <v>44393</v>
       </c>
@@ -1701,10 +1698,10 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="2">
         <v>44393</v>
       </c>
@@ -1836,10 +1833,10 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="2">
         <v>44394</v>
       </c>
@@ -1968,10 +1965,10 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="2">
         <v>44395</v>
       </c>
@@ -2074,7 +2071,7 @@
       <c r="C25" s="2">
         <v>44395</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E25">
@@ -2100,14 +2097,14 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="3"/>
       <c r="C26" s="2">
         <v>44395</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E26">
@@ -2232,10 +2229,10 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="2">
         <v>44396</v>
       </c>
@@ -2364,10 +2361,10 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="4"/>
+      <c r="B34" s="3"/>
       <c r="C34" s="2">
         <v>44396</v>
       </c>
@@ -2496,10 +2493,10 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="4"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="2">
         <v>44397</v>
       </c>
@@ -2628,10 +2625,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="3"/>
       <c r="C42" s="2">
         <v>44398</v>
       </c>
@@ -2760,10 +2757,10 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" s="4"/>
+      <c r="B46" s="3"/>
       <c r="C46" s="2">
         <v>44398</v>
       </c>
@@ -2892,10 +2889,10 @@
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" s="4"/>
+      <c r="B50" s="3"/>
       <c r="C50" s="2">
         <v>44398</v>
       </c>
@@ -2977,7 +2974,7 @@
       <c r="F52">
         <v>1</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" t="s">
         <v>52</v>
       </c>
       <c r="H52" t="s">
@@ -3027,10 +3024,10 @@
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54" s="4"/>
+      <c r="B54" s="3"/>
       <c r="C54" s="2">
         <v>44399</v>
       </c>
@@ -3159,10 +3156,10 @@
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58" s="4"/>
+      <c r="B58" s="3"/>
       <c r="C58" s="2">
         <v>44399</v>
       </c>
@@ -3291,10 +3288,10 @@
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62" s="4"/>
+      <c r="B62" s="3"/>
       <c r="C62" s="2">
         <v>44399</v>
       </c>
@@ -3652,6 +3649,52 @@
       <c r="K72">
         <v>151.833236694335</v>
       </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="5"/>
+      <c r="B75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="G75" s="5"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="5"/>
+      <c r="B76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="G76" s="5"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="5"/>
+      <c r="B77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="G77" s="5"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="5"/>
+      <c r="B78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="G78" s="5"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="5"/>
+      <c r="B79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="G79" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0100-000000000000}">

</xml_diff>